<commit_message>
adding robot framework files
</commit_message>
<xml_diff>
--- a/root/data/ParabankData.xlsx
+++ b/root/data/ParabankData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse\eclipse-jee-2023-03-R-win32-x86_64\API\python_selenium_robot_framework\root\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse\eclipse-jee-2023-03-R-win32-x86_64\API\python_selen_robot_framework_parabank\root\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1A2C40-D9DE-46FF-AA8E-6F972FE245C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA35D7E3-E080-4809-B990-587A772D40DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1F4F56B-1BB9-4A3E-91A8-12372D1ECCFB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
   <si>
     <t>Address</t>
   </si>
@@ -123,7 +123,145 @@
     <t>SAVINGS</t>
   </si>
   <si>
-    <t>Account_Number</t>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>123 Main St</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>212-555-7890</t>
+  </si>
+  <si>
+    <t>123-45-6789</t>
+  </si>
+  <si>
+    <t>johndoe92</t>
+  </si>
+  <si>
+    <t>Pass@1234</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>456 Oak Avenue</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>312-555-2345</t>
+  </si>
+  <si>
+    <t>234-56-7890</t>
+  </si>
+  <si>
+    <t>emilys88</t>
+  </si>
+  <si>
+    <t>MySecurePwd1</t>
+  </si>
+  <si>
+    <t>Checking</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>789 Pine Street</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>713-555-6789</t>
+  </si>
+  <si>
+    <t>345-67-8901</t>
+  </si>
+  <si>
+    <t>mjohnson76</t>
+  </si>
+  <si>
+    <t>Secure#Pass2</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>321 Maple Drive</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>305-555-8901</t>
+  </si>
+  <si>
+    <t>456-78-9012</t>
+  </si>
+  <si>
+    <t>sbrown90</t>
+  </si>
+  <si>
+    <t>Test@Pass99</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>987 Cedar Lane</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>206-555-3456</t>
+  </si>
+  <si>
+    <t>567-89-0123</t>
+  </si>
+  <si>
+    <t>wtaylor85</t>
+  </si>
+  <si>
+    <t>P@ssword123</t>
   </si>
 </sst>
 </file>
@@ -191,7 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -204,6 +342,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -520,28 +661,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C61DC5F-FB77-45AF-9DB5-EF7ACC109C9A}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="15.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" style="1"/>
-    <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="11" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -578,11 +721,8 @@
       <c r="L1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -619,11 +759,8 @@
       <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="2">
-        <v>22890</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -660,11 +797,8 @@
       <c r="L3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="2">
-        <v>58795</v>
-      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -701,8 +835,195 @@
       <c r="L4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="2">
-        <v>45855</v>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="5">
+        <v>10001</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="5">
+        <v>60614</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="5">
+        <v>77002</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="5">
+        <v>33101</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="5">
+        <v>98101</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>